<commit_message>
Added more documentation to the README
</commit_message>
<xml_diff>
--- a/docs/TPCape_RevA_BOM.xlsx
+++ b/docs/TPCape_RevA_BOM.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\pru-printer\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="5970" windowHeight="5670" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="5970" windowHeight="5670" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TPcape_BOM" sheetId="4" r:id="rId1"/>
@@ -12,12 +17,12 @@
     <sheet name="interface" sheetId="6" r:id="rId3"/>
     <sheet name="motor" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="324">
   <si>
     <t>Capture CIS Standard Bill Of Materials - Standard Report</t>
   </si>
@@ -577,9 +582,6 @@
     <t>VDD_5V</t>
   </si>
   <si>
-    <t>Tpcape</t>
-  </si>
-  <si>
     <t>Vcc2</t>
   </si>
   <si>
@@ -983,17 +985,26 @@
   </si>
   <si>
     <t>Cape Signal</t>
+  </si>
+  <si>
+    <t>Interface board</t>
+  </si>
+  <si>
+    <t>Translation?</t>
+  </si>
+  <si>
+    <t>TPcape</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="g"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1205,7 +1216,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1237,9 +1248,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1271,6 +1283,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1446,14 +1459,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" customWidth="1"/>
     <col min="2" max="2" width="4.5703125" bestFit="1" customWidth="1"/>
@@ -1470,7 +1483,7 @@
     <col min="13" max="13" width="62.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1480,7 +1493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1491,27 +1504,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1552,7 +1565,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -1579,7 +1592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -1606,7 +1619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>3</v>
       </c>
@@ -1645,7 +1658,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>4</v>
       </c>
@@ -1684,7 +1697,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>5</v>
       </c>
@@ -1713,7 +1726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>6</v>
       </c>
@@ -1753,7 +1766,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>7</v>
       </c>
@@ -1771,7 +1784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>8</v>
       </c>
@@ -1789,7 +1802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>9</v>
       </c>
@@ -1807,24 +1820,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>10</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I18" t="s">
         <v>35</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K18" s="6">
         <v>0.14000000000000001</v>
@@ -1834,7 +1847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>11</v>
       </c>
@@ -1842,19 +1855,19 @@
         <v>1</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I19" t="s">
         <v>35</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K19" s="6">
         <v>0.73</v>
@@ -1864,7 +1877,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>12</v>
       </c>
@@ -1873,7 +1886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>13</v>
       </c>
@@ -1882,7 +1895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>14</v>
       </c>
@@ -1891,7 +1904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>15</v>
       </c>
@@ -1900,7 +1913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>16</v>
       </c>
@@ -1909,124 +1922,124 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D25" t="s">
+        <v>293</v>
+      </c>
+      <c r="E25" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="E25" s="13" t="s">
-        <v>295</v>
-      </c>
       <c r="G25" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L25" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>18</v>
       </c>
       <c r="C26" t="s">
+        <v>270</v>
+      </c>
+      <c r="D26" t="s">
+        <v>275</v>
+      </c>
+      <c r="E26" t="s">
+        <v>276</v>
+      </c>
+      <c r="F26" t="s">
+        <v>272</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>271</v>
-      </c>
-      <c r="D26" t="s">
-        <v>276</v>
-      </c>
-      <c r="E26" t="s">
-        <v>277</v>
-      </c>
-      <c r="F26" t="s">
-        <v>273</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>272</v>
       </c>
       <c r="L26" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D27" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E27" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F27" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L27" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D28" t="s">
+        <v>221</v>
+      </c>
+      <c r="E28" t="s">
         <v>222</v>
       </c>
-      <c r="E28" t="s">
-        <v>223</v>
-      </c>
       <c r="F28" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="L28" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D29" t="s">
+        <v>246</v>
+      </c>
+      <c r="E29" t="s">
         <v>247</v>
       </c>
-      <c r="E29" t="s">
-        <v>248</v>
-      </c>
       <c r="F29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L29" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>22</v>
       </c>
@@ -2035,186 +2048,186 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D31">
         <v>12</v>
       </c>
       <c r="E31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F31" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="L31" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>24</v>
       </c>
       <c r="C32" t="s">
+        <v>235</v>
+      </c>
+      <c r="D32" t="s">
+        <v>249</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="F32" t="s">
+        <v>241</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>236</v>
-      </c>
-      <c r="D32" t="s">
-        <v>250</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="F32" t="s">
-        <v>242</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>237</v>
       </c>
       <c r="L32" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>25</v>
       </c>
       <c r="C33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D33" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F33" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>26</v>
       </c>
       <c r="C34" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D34" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E34" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F34" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>27</v>
       </c>
       <c r="C35" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D35" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E35" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F35" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>28</v>
       </c>
       <c r="C36" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D36">
         <v>180</v>
       </c>
       <c r="E36" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F36" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>29</v>
       </c>
       <c r="C37" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D37" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F37" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>31</v>
       </c>
       <c r="C39" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>25</v>
       </c>
@@ -2266,14 +2279,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H10" sqref="H10:J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" customWidth="1"/>
     <col min="3" max="3" width="3.85546875" bestFit="1" customWidth="1"/>
@@ -2283,12 +2296,12 @@
     <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -2308,7 +2321,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -2331,7 +2344,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -2351,10 +2364,10 @@
         <v>100</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -2373,7 +2386,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -2399,10 +2412,10 @@
         <v>138</v>
       </c>
       <c r="J7" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -2428,10 +2441,10 @@
         <v>158</v>
       </c>
       <c r="J8" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -2451,7 +2464,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -2474,13 +2487,13 @@
         <v>71</v>
       </c>
       <c r="I10" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="J10" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="J10" s="8" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -2500,7 +2513,7 @@
         <v>105</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>174</v>
@@ -2509,10 +2522,10 @@
         <v>147</v>
       </c>
       <c r="J11" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>9</v>
       </c>
@@ -2538,10 +2551,10 @@
         <v>148</v>
       </c>
       <c r="J12" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>10</v>
       </c>
@@ -2567,10 +2580,10 @@
         <v>149</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>11</v>
       </c>
@@ -2596,10 +2609,10 @@
         <v>159</v>
       </c>
       <c r="J14" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>12</v>
       </c>
@@ -2625,10 +2638,10 @@
         <v>161</v>
       </c>
       <c r="J15" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>13</v>
       </c>
@@ -2654,10 +2667,10 @@
         <v>140</v>
       </c>
       <c r="J16" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>14</v>
       </c>
@@ -2679,10 +2692,10 @@
         <v>139</v>
       </c>
       <c r="J17" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>15</v>
       </c>
@@ -2704,10 +2717,10 @@
         <v>141</v>
       </c>
       <c r="J18" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>16</v>
       </c>
@@ -2733,10 +2746,10 @@
         <v>142</v>
       </c>
       <c r="J19" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>17</v>
       </c>
@@ -2762,10 +2775,10 @@
         <v>143</v>
       </c>
       <c r="J20" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>18</v>
       </c>
@@ -2791,10 +2804,10 @@
         <v>144</v>
       </c>
       <c r="J21" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>19</v>
       </c>
@@ -2820,10 +2833,10 @@
         <v>145</v>
       </c>
       <c r="J22" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>20</v>
       </c>
@@ -2849,10 +2862,10 @@
         <v>146</v>
       </c>
       <c r="J23" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>21</v>
       </c>
@@ -2881,7 +2894,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>22</v>
       </c>
@@ -2910,7 +2923,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>23</v>
       </c>
@@ -2939,7 +2952,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>24</v>
       </c>
@@ -2968,7 +2981,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>25</v>
       </c>
@@ -2995,7 +3008,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>26</v>
       </c>
@@ -3020,7 +3033,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>27</v>
       </c>
@@ -3049,7 +3062,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>28</v>
       </c>
@@ -3078,7 +3091,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>29</v>
       </c>
@@ -3107,7 +3120,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>30</v>
       </c>
@@ -3136,7 +3149,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>1</v>
       </c>
@@ -3156,10 +3169,10 @@
         <v>122</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>2</v>
       </c>
@@ -3176,7 +3189,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>3</v>
       </c>
@@ -3199,7 +3212,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>4</v>
       </c>
@@ -3219,7 +3232,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>5</v>
       </c>
@@ -3239,7 +3252,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <v>6</v>
       </c>
@@ -3259,7 +3272,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>7</v>
       </c>
@@ -3279,7 +3292,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <v>8</v>
       </c>
@@ -3290,95 +3303,95 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E47" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3</v>
       </c>
       <c r="B48" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E48" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>4</v>
       </c>
       <c r="B49" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E49" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E50" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E51" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E52" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2</v>
       </c>
       <c r="B53" t="s">
+        <v>267</v>
+      </c>
+      <c r="E53" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54" t="s">
         <v>268</v>
       </c>
-      <c r="E53" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54">
-        <v>1</v>
-      </c>
-      <c r="B54" t="s">
-        <v>269</v>
-      </c>
       <c r="E54" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <f>SUM(A47:A52)</f>
         <v>20</v>
@@ -3390,31 +3403,35 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="12" max="12" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13">
-      <c r="B2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>323</v>
+      </c>
+      <c r="E2" t="s">
+        <v>322</v>
+      </c>
+      <c r="I2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>68</v>
       </c>
       <c r="B3" t="s">
         <v>69</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="8" t="s">
         <v>70</v>
       </c>
       <c r="E3" t="s">
@@ -3423,7 +3440,7 @@
       <c r="F3" t="s">
         <v>69</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="8" t="s">
         <v>70</v>
       </c>
       <c r="I3" t="s">
@@ -3432,14 +3449,14 @@
       <c r="J3" t="s">
         <v>69</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="8" t="s">
         <v>70</v>
       </c>
       <c r="L3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -3453,25 +3470,25 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>195</v>
-      </c>
-      <c r="G4" t="s">
+        <v>194</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>96</v>
       </c>
       <c r="I4" s="9">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>195</v>
-      </c>
-      <c r="K4" t="s">
+        <v>194</v>
+      </c>
+      <c r="K4" s="8" t="s">
         <v>96</v>
       </c>
       <c r="L4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -3485,28 +3502,28 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>187</v>
-      </c>
-      <c r="G5" t="s">
+        <v>186</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I5" s="9">
         <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>187</v>
-      </c>
-      <c r="K5" t="s">
+        <v>186</v>
+      </c>
+      <c r="K5" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M5" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -3520,28 +3537,28 @@
         <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>188</v>
-      </c>
-      <c r="G6" t="s">
+        <v>187</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>98</v>
       </c>
       <c r="I6" s="9">
         <v>3</v>
       </c>
       <c r="J6" t="s">
-        <v>188</v>
-      </c>
-      <c r="K6" t="s">
+        <v>187</v>
+      </c>
+      <c r="K6" s="8" t="s">
         <v>98</v>
       </c>
       <c r="L6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M6" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -3557,23 +3574,23 @@
       <c r="F7" t="s">
         <v>77</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I7" s="9">
         <v>4</v>
       </c>
       <c r="J7" t="s">
-        <v>189</v>
-      </c>
-      <c r="K7" t="s">
+        <v>188</v>
+      </c>
+      <c r="K7" s="8" t="s">
         <v>98</v>
       </c>
       <c r="L7" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -3589,23 +3606,23 @@
       <c r="F8" t="s">
         <v>77</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I8" s="9">
         <v>5</v>
       </c>
       <c r="J8" t="s">
-        <v>190</v>
-      </c>
-      <c r="K8" t="s">
+        <v>189</v>
+      </c>
+      <c r="K8" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L8" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -3619,9 +3636,9 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>191</v>
-      </c>
-      <c r="G9" t="s">
+        <v>190</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I9" s="9">
@@ -3630,14 +3647,14 @@
       <c r="J9" t="s">
         <v>77</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L9" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -3651,9 +3668,9 @@
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>192</v>
-      </c>
-      <c r="G10" t="s">
+        <v>191</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I10" s="9">
@@ -3662,11 +3679,11 @@
       <c r="J10" t="s">
         <v>77</v>
       </c>
-      <c r="K10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="K10" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -3682,23 +3699,23 @@
       <c r="F11" t="s">
         <v>80</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="8" t="s">
         <v>96</v>
       </c>
       <c r="I11" s="9">
         <v>8</v>
       </c>
       <c r="J11" t="s">
-        <v>191</v>
-      </c>
-      <c r="K11" t="s">
+        <v>190</v>
+      </c>
+      <c r="K11" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L11" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>9</v>
       </c>
@@ -3714,23 +3731,23 @@
       <c r="F12" t="s">
         <v>80</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="8" t="s">
         <v>96</v>
       </c>
       <c r="I12" s="9">
         <v>9</v>
       </c>
       <c r="J12" t="s">
-        <v>192</v>
-      </c>
-      <c r="K12" t="s">
+        <v>191</v>
+      </c>
+      <c r="K12" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L12" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>10</v>
       </c>
@@ -3746,7 +3763,7 @@
       <c r="F13" t="s">
         <v>81</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I13" s="9">
@@ -3755,14 +3772,14 @@
       <c r="J13" t="s">
         <v>80</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="8" t="s">
         <v>96</v>
       </c>
       <c r="L13" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>11</v>
       </c>
@@ -3778,7 +3795,7 @@
       <c r="F14" t="s">
         <v>82</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I14" s="9">
@@ -3787,14 +3804,14 @@
       <c r="J14" t="s">
         <v>80</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="8" t="s">
         <v>96</v>
       </c>
       <c r="L14" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>12</v>
       </c>
@@ -3810,7 +3827,7 @@
       <c r="F15" t="s">
         <v>83</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I15" s="9">
@@ -3819,14 +3836,14 @@
       <c r="J15" t="s">
         <v>81</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L15" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>13</v>
       </c>
@@ -3840,9 +3857,9 @@
         <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>190</v>
-      </c>
-      <c r="G16" t="s">
+        <v>189</v>
+      </c>
+      <c r="G16" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I16" s="9">
@@ -3851,14 +3868,14 @@
       <c r="J16" t="s">
         <v>82</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L16" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>14</v>
       </c>
@@ -3872,7 +3889,7 @@
         <v>16</v>
       </c>
       <c r="F17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>98</v>
@@ -3883,14 +3900,14 @@
       <c r="J17" t="s">
         <v>83</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L17" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>15</v>
       </c>
@@ -3904,22 +3921,22 @@
         <v>17</v>
       </c>
       <c r="F18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I18" s="9">
         <v>15</v>
       </c>
       <c r="J18" t="s">
-        <v>190</v>
-      </c>
-      <c r="K18" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>189</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>16</v>
       </c>
@@ -3935,23 +3952,23 @@
       <c r="F19" t="s">
         <v>86</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I19" s="9">
         <v>16</v>
       </c>
       <c r="J19" t="s">
-        <v>300</v>
-      </c>
-      <c r="K19" t="s">
+        <v>299</v>
+      </c>
+      <c r="K19" s="8" t="s">
         <v>98</v>
       </c>
       <c r="L19" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>17</v>
       </c>
@@ -3967,23 +3984,23 @@
       <c r="F20" t="s">
         <v>87</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I20" s="9">
         <v>17</v>
       </c>
       <c r="J20" t="s">
-        <v>193</v>
-      </c>
-      <c r="K20" t="s">
-        <v>301</v>
+        <v>192</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>300</v>
       </c>
       <c r="L20" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>18</v>
       </c>
@@ -3999,7 +4016,7 @@
       <c r="F21" t="s">
         <v>88</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I21" s="9">
@@ -4008,14 +4025,14 @@
       <c r="J21" t="s">
         <v>86</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L21" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>19</v>
       </c>
@@ -4031,7 +4048,7 @@
       <c r="F22" t="s">
         <v>80</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="8" t="s">
         <v>96</v>
       </c>
       <c r="I22" s="9">
@@ -4040,14 +4057,14 @@
       <c r="J22" t="s">
         <v>87</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L22" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>20</v>
       </c>
@@ -4063,7 +4080,7 @@
       <c r="F23" t="s">
         <v>80</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="8" t="s">
         <v>96</v>
       </c>
       <c r="I23" s="9">
@@ -4072,14 +4089,14 @@
       <c r="J23" t="s">
         <v>88</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L23" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>21</v>
       </c>
@@ -4093,9 +4110,9 @@
         <v>23</v>
       </c>
       <c r="F24" t="s">
-        <v>194</v>
-      </c>
-      <c r="G24" t="s">
+        <v>193</v>
+      </c>
+      <c r="G24" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I24" s="9">
@@ -4104,14 +4121,14 @@
       <c r="J24" t="s">
         <v>80</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" s="8" t="s">
         <v>96</v>
       </c>
       <c r="L24" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>22</v>
       </c>
@@ -4127,7 +4144,7 @@
       <c r="F25" t="s">
         <v>78</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="8" t="s">
         <v>98</v>
       </c>
       <c r="I25" s="9">
@@ -4136,14 +4153,14 @@
       <c r="J25" t="s">
         <v>80</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" s="8" t="s">
         <v>96</v>
       </c>
       <c r="L25" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>23</v>
       </c>
@@ -4159,23 +4176,23 @@
       <c r="F26" t="s">
         <v>77</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I26" s="9">
         <v>23</v>
       </c>
       <c r="J26" t="s">
-        <v>194</v>
-      </c>
-      <c r="K26" t="s">
+        <v>193</v>
+      </c>
+      <c r="K26" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L26" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>24</v>
       </c>
@@ -4191,7 +4208,7 @@
       <c r="F27" t="s">
         <v>77</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I27" s="9">
@@ -4200,14 +4217,14 @@
       <c r="J27" t="s">
         <v>78</v>
       </c>
-      <c r="K27" t="s">
+      <c r="K27" s="8" t="s">
         <v>98</v>
       </c>
       <c r="L27" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>25</v>
       </c>
@@ -4221,9 +4238,9 @@
         <v>5</v>
       </c>
       <c r="F28" t="s">
-        <v>190</v>
-      </c>
-      <c r="G28" t="s">
+        <v>189</v>
+      </c>
+      <c r="G28" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I28" s="9">
@@ -4232,11 +4249,11 @@
       <c r="J28" t="s">
         <v>77</v>
       </c>
-      <c r="K28" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="K28" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>26</v>
       </c>
@@ -4250,9 +4267,9 @@
         <v>4</v>
       </c>
       <c r="F29" t="s">
-        <v>189</v>
-      </c>
-      <c r="G29" t="s">
+        <v>188</v>
+      </c>
+      <c r="G29" s="8" t="s">
         <v>98</v>
       </c>
       <c r="I29" s="9">
@@ -4261,14 +4278,14 @@
       <c r="J29" t="s">
         <v>77</v>
       </c>
-      <c r="K29" t="s">
+      <c r="K29" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L29" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>27</v>
       </c>
@@ -4284,7 +4301,7 @@
       <c r="F30" t="s">
         <v>92</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I30" s="9">
@@ -4293,14 +4310,14 @@
       <c r="J30" t="s">
         <v>92</v>
       </c>
-      <c r="K30" t="s">
+      <c r="K30" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L30" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>28</v>
       </c>
@@ -4316,7 +4333,7 @@
       <c r="F31" t="s">
         <v>93</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I31" s="9">
@@ -4325,14 +4342,14 @@
       <c r="J31" t="s">
         <v>93</v>
       </c>
-      <c r="K31" t="s">
+      <c r="K31" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L31" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>29</v>
       </c>
@@ -4348,7 +4365,7 @@
       <c r="F32" t="s">
         <v>94</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I32" s="9">
@@ -4357,14 +4374,14 @@
       <c r="J32" t="s">
         <v>94</v>
       </c>
-      <c r="K32" t="s">
+      <c r="K32" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L32" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>30</v>
       </c>
@@ -4380,7 +4397,7 @@
       <c r="F33" t="s">
         <v>95</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I33" s="9">
@@ -4389,14 +4406,22 @@
       <c r="J33" t="s">
         <v>95</v>
       </c>
-      <c r="K33" t="s">
+      <c r="K33" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L33" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G34" s="8"/>
+      <c r="K34" s="8"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G35" s="8"/>
+      <c r="K35" s="8"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>1</v>
       </c>
@@ -4410,25 +4435,25 @@
         <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>187</v>
-      </c>
-      <c r="G36" t="s">
+        <v>186</v>
+      </c>
+      <c r="G36" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I36" s="9">
         <v>1</v>
       </c>
       <c r="J36" t="s">
-        <v>187</v>
-      </c>
-      <c r="K36" t="s">
+        <v>186</v>
+      </c>
+      <c r="K36" s="8" t="s">
         <v>97</v>
       </c>
       <c r="L36" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>2</v>
       </c>
@@ -4438,20 +4463,21 @@
       <c r="C37" s="9" t="s">
         <v>98</v>
       </c>
+      <c r="G37" s="8"/>
       <c r="I37" s="9">
         <v>2</v>
       </c>
       <c r="J37" t="s">
-        <v>196</v>
-      </c>
-      <c r="K37" t="s">
+        <v>195</v>
+      </c>
+      <c r="K37" s="8" t="s">
         <v>98</v>
       </c>
       <c r="L37" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>3</v>
       </c>
@@ -4461,20 +4487,21 @@
       <c r="C38" s="9" t="s">
         <v>96</v>
       </c>
+      <c r="G38" s="8"/>
       <c r="I38" s="9">
         <v>3</v>
       </c>
       <c r="J38" t="s">
-        <v>197</v>
-      </c>
-      <c r="K38" t="s">
+        <v>196</v>
+      </c>
+      <c r="K38" s="8" t="s">
         <v>98</v>
       </c>
       <c r="L38" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>4</v>
       </c>
@@ -4488,22 +4515,22 @@
         <v>4</v>
       </c>
       <c r="F39" t="s">
-        <v>198</v>
-      </c>
-      <c r="G39" t="s">
+        <v>197</v>
+      </c>
+      <c r="G39" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I39" s="9">
         <v>4</v>
       </c>
       <c r="J39" t="s">
-        <v>198</v>
-      </c>
-      <c r="K39" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12">
+        <v>197</v>
+      </c>
+      <c r="K39" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>5</v>
       </c>
@@ -4517,22 +4544,22 @@
         <v>5</v>
       </c>
       <c r="F40" t="s">
-        <v>199</v>
-      </c>
-      <c r="G40" t="s">
+        <v>198</v>
+      </c>
+      <c r="G40" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I40" s="9">
         <v>5</v>
       </c>
       <c r="J40" t="s">
-        <v>199</v>
-      </c>
-      <c r="K40" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12">
+        <v>198</v>
+      </c>
+      <c r="K40" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <v>6</v>
       </c>
@@ -4546,22 +4573,22 @@
         <v>6</v>
       </c>
       <c r="F41" t="s">
-        <v>200</v>
-      </c>
-      <c r="G41" t="s">
+        <v>199</v>
+      </c>
+      <c r="G41" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I41" s="9">
         <v>6</v>
       </c>
       <c r="J41" t="s">
-        <v>200</v>
-      </c>
-      <c r="K41" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12">
+        <v>199</v>
+      </c>
+      <c r="K41" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>7</v>
       </c>
@@ -4575,22 +4602,22 @@
         <v>7</v>
       </c>
       <c r="F42" t="s">
-        <v>201</v>
-      </c>
-      <c r="G42" t="s">
+        <v>200</v>
+      </c>
+      <c r="G42" s="8" t="s">
         <v>97</v>
       </c>
       <c r="I42" s="9">
         <v>7</v>
       </c>
       <c r="J42" t="s">
-        <v>201</v>
-      </c>
-      <c r="K42" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12">
+        <v>200</v>
+      </c>
+      <c r="K42" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <v>8</v>
       </c>
@@ -4600,12 +4627,14 @@
       <c r="C43" s="9" t="s">
         <v>96</v>
       </c>
+      <c r="G43" s="8"/>
       <c r="I43" s="9">
         <v>8</v>
       </c>
       <c r="J43" t="s">
         <v>121</v>
       </c>
+      <c r="K43" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4614,45 +4643,45 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B1" t="s">
         <v>255</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>256</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>257</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>258</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>259</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>260</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>261</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>262</v>
       </c>
-      <c r="K1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4681,7 +4710,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4710,7 +4739,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4739,7 +4768,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -4768,7 +4797,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -4797,7 +4826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -4826,7 +4855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -4855,7 +4884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -4884,7 +4913,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
         <v>93</v>
       </c>
@@ -4898,7 +4927,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -4927,7 +4956,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -4956,7 +4985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -4985,7 +5014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>

</xml_diff>